<commit_message>
Mad the changes in webActionPage& created sepreate pages for JobDetalsand Propose Compensation,etc under commonpage folder.
</commit_message>
<xml_diff>
--- a/Data/testData.xlsx
+++ b/Data/testData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="143">
   <si>
     <t xml:space="preserve">Serial </t>
   </si>
@@ -262,10 +262,10 @@
     <t>Slovakia</t>
   </si>
   <si>
-    <t>Damien</t>
-  </si>
-  <si>
-    <t>Beatty</t>
+    <t>Cleve</t>
+  </si>
+  <si>
+    <t>Fay</t>
   </si>
   <si>
     <t>041/562 66 84</t>
@@ -406,31 +406,34 @@
     <t>Vseobecna zdrav. Poist</t>
   </si>
   <si>
+    <t>{"name":"TimeoutError"}</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Isabell</t>
+  </si>
+  <si>
+    <t>Beahan</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Destin</t>
+  </si>
+  <si>
+    <t>Nader</t>
+  </si>
+  <si>
     <t>{"name":"Error"}</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Isabell</t>
-  </si>
-  <si>
-    <t>Beahan</t>
-  </si>
-  <si>
-    <t>{}</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Destin</t>
-  </si>
-  <si>
-    <t>Nader</t>
   </si>
   <si>
     <t>Test4</t>
@@ -1829,7 +1832,7 @@
         <v>129</v>
       </c>
       <c r="CE4" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="CF4" s="15" t="s">
         <v>131</v>
@@ -1837,7 +1840,7 @@
     </row>
     <row r="5" ht="14.4" customHeight="1" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>80</v>
@@ -1846,10 +1849,10 @@
         <v>81</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>84</v>

</xml_diff>